<commit_message>
adicao dos custos ao kmeans e atualizacao setup experimental
</commit_message>
<xml_diff>
--- a/template_dados_analiticos.xlsx
+++ b/template_dados_analiticos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
   <si>
     <t xml:space="preserve">atribuições</t>
   </si>
@@ -35,18 +35,27 @@
     <t xml:space="preserve">'colocar formula de a(n,k) no bloco de incialização</t>
   </si>
   <si>
+    <t xml:space="preserve">Nºcores*(12+17*Nºclusters)+6*Nºpixels+13</t>
+  </si>
+  <si>
     <t xml:space="preserve">operações</t>
   </si>
   <si>
     <t xml:space="preserve">colocar formula de o(n,k) no bloco de incialização</t>
   </si>
   <si>
+    <t xml:space="preserve">Nºcores*(6*Nºclusters+1)+Nºpixels</t>
+  </si>
+  <si>
     <t xml:space="preserve">comparações</t>
   </si>
   <si>
     <t xml:space="preserve">colocar formula de c(n,k) no bloco de incialização</t>
   </si>
   <si>
+    <t xml:space="preserve">Nºcores*(Nºclusters+1)=Nºpixels</t>
+  </si>
+  <si>
     <t xml:space="preserve">Custo (norma L1)</t>
   </si>
   <si>
@@ -113,10 +122,66 @@
     <t xml:space="preserve">'colocar formula de a(n,k) no bloco iterativo</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nºiterações*(Nºcores*(10*Nºpixels+11*Nºclusters*Nºpixels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">+12*Nºclusters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">+15*Nºclusters+14*Nºclusters*Nºpixels+13*Nºpixels+15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">colocar formula de o(n,k) no bloco iterativo</t>
   </si>
   <si>
+    <t xml:space="preserve">Nºiterações*(Nºcores*(3*Nºclusters*Nºpixels+2*Nºpixels+2*Nºclusters)+Nºclusters*Nºpixels+4*Nºclusters+7*Nºpixels+1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">colocar formula de c(n,k) no bloco iterativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nºiterações*(Nºcores*(Nºclusters*Nºpixels+Nºclusters+Nºpixels)+2*(Nºclusters+Nºpixels)+3*(Nºclusters+Nºpixels)+1)</t>
   </si>
   <si>
     <t xml:space="preserve">Iterações/Cluster</t>
@@ -192,7 +257,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -352,6 +417,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -596,7 +667,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -621,8 +692,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -645,15 +720,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,7 +836,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1193,11 +1268,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="26321081"/>
-        <c:axId val="48241426"/>
+        <c:axId val="99792193"/>
+        <c:axId val="37599046"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="26321081"/>
+        <c:axId val="99792193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,12 +1338,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48241426"/>
+        <c:crossAx val="37599046"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48241426"/>
+        <c:axId val="37599046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1419,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26321081"/>
+        <c:crossAx val="99792193"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1371,7 +1446,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1767,11 +1842,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="68051888"/>
-        <c:axId val="91347179"/>
+        <c:axId val="82878191"/>
+        <c:axId val="48661533"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68051888"/>
+        <c:axId val="82878191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1838,13 +1913,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91347179"/>
+        <c:crossAx val="48661533"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91347179"/>
+        <c:axId val="48661533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1920,7 +1995,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68051888"/>
+        <c:crossAx val="82878191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1947,7 +2022,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2023,6 +2098,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2059,16 +2135,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67926410</c:v>
+                  <c:v>70215950</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58249686</c:v>
+                  <c:v>60213090</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58218985</c:v>
+                  <c:v>60181297</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23349955</c:v>
+                  <c:v>24136975</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,6 +2183,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2143,16 +2220,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>89678330</c:v>
+                  <c:v>93112640</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140988463</c:v>
+                  <c:v>146387824</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62887392</c:v>
+                  <c:v>65295684</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61654580</c:v>
+                  <c:v>64015640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,6 +2282,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2223,6 +2301,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2259,16 +2338,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>167145375</c:v>
+                  <c:v>174013995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>350371670</c:v>
+                  <c:v>364769966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112870433</c:v>
+                  <c:v>117508625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99592025</c:v>
+                  <c:v>103684529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2307,6 +2386,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2343,27 +2423,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>253046123</c:v>
+                  <c:v>263921438</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>228418044</c:v>
+                  <c:v>238235064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145280716</c:v>
+                  <c:v>151524436</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82407528</c:v>
+                  <c:v>85949118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2805384"/>
-        <c:axId val="49546033"/>
+        <c:axId val="46250067"/>
+        <c:axId val="66303047"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2805384"/>
+        <c:axId val="46250067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2429,13 +2509,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49546033"/>
+        <c:crossAx val="66303047"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10000"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49546033"/>
+        <c:axId val="66303047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2591,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2805384"/>
+        <c:crossAx val="46250067"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2538,7 +2618,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2651,16 +2731,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>67926410</c:v>
+                  <c:v>70215950</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89678330</c:v>
+                  <c:v>93112640</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>167145375</c:v>
+                  <c:v>174013995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>253046123</c:v>
+                  <c:v>263921438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2736,16 +2816,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>58249686</c:v>
+                  <c:v>60213090</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140988463</c:v>
+                  <c:v>146387824</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>350371670</c:v>
+                  <c:v>364769966</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>228418044</c:v>
+                  <c:v>238235064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2821,16 +2901,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>58218985</c:v>
+                  <c:v>60181297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62887392</c:v>
+                  <c:v>65295684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112870433</c:v>
+                  <c:v>117508625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145280716</c:v>
+                  <c:v>151524436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2939,27 +3019,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>23349955</c:v>
+                  <c:v>24136975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61654580</c:v>
+                  <c:v>64015640</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99592025</c:v>
+                  <c:v>103684529</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82407528</c:v>
+                  <c:v>85949118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="87519426"/>
-        <c:axId val="68648077"/>
+        <c:axId val="82471256"/>
+        <c:axId val="50411862"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87519426"/>
+        <c:axId val="82471256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -3027,13 +3107,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68648077"/>
+        <c:crossAx val="50411862"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68648077"/>
+        <c:axId val="50411862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,7 +3189,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87519426"/>
+        <c:crossAx val="82471256"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3141,13 +3221,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>202320</xdr:colOff>
+      <xdr:colOff>202680</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
@@ -3157,8 +3237,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7371360" y="258480"/>
-        <a:ext cx="4481640" cy="4106880"/>
+        <a:off x="7504920" y="258840"/>
+        <a:ext cx="4481280" cy="4106520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3173,11 +3253,11 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>667080</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>292680</xdr:colOff>
+      <xdr:colOff>292320</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
@@ -3187,8 +3267,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11995200" y="246240"/>
-        <a:ext cx="4454280" cy="4194360"/>
+        <a:off x="12128760" y="246600"/>
+        <a:ext cx="4449960" cy="4194000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3212,9 +3292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>646560</xdr:colOff>
+      <xdr:colOff>646200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3223,7 +3303,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8645760" y="239400"/>
-        <a:ext cx="4781880" cy="4038480"/>
+        <a:ext cx="4781520" cy="4038120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3242,9 +3322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>653400</xdr:colOff>
+      <xdr:colOff>653040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3252,8 +3332,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14104080" y="246600"/>
-        <a:ext cx="4659480" cy="4125960"/>
+        <a:off x="14103720" y="246600"/>
+        <a:ext cx="4654440" cy="4125600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3274,14 +3354,14 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="9.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="10.75"/>
   </cols>
   <sheetData>
@@ -3364,6 +3444,9 @@
         <f aca="false">3*(12+17*E$3)+6*$A$5+13</f>
         <v>327544</v>
       </c>
+      <c r="F5" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
@@ -3409,7 +3492,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3463,7 +3546,7 @@
         <v>38253</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3486,6 +3569,9 @@
         <f aca="false">3*(6*E$10+1)+$A12</f>
         <v>54633</v>
       </c>
+      <c r="F12" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
@@ -3531,7 +3617,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -3585,7 +3671,7 @@
         <v>38178</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,6 +3694,9 @@
         <f aca="false">3*(E$17+1)+$A19</f>
         <v>54558</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
@@ -3653,7 +3742,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3690,19 +3779,19 @@
       <c r="A26" s="5" t="n">
         <v>38160</v>
       </c>
-      <c r="B26" s="7" t="n">
+      <c r="B26" s="8" t="n">
         <f aca="false">B4+B11+B18</f>
         <v>305479</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="8" t="n">
         <f aca="false">C4+C11+C18</f>
         <v>305551</v>
       </c>
-      <c r="D26" s="7" t="n">
+      <c r="D26" s="8" t="n">
         <f aca="false">D4+D11+D18</f>
         <v>305623</v>
       </c>
-      <c r="E26" s="7" t="n">
+      <c r="E26" s="8" t="n">
         <f aca="false">E4+E11+E18</f>
         <v>305695</v>
       </c>
@@ -3711,19 +3800,19 @@
       <c r="A27" s="5" t="n">
         <v>54540</v>
       </c>
-      <c r="B27" s="7" t="n">
+      <c r="B27" s="8" t="n">
         <f aca="false">B5+B12+B19</f>
         <v>436519</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="8" t="n">
         <f aca="false">C5+C12+C19</f>
         <v>436591</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="8" t="n">
         <f aca="false">D5+D12+D19</f>
         <v>436663</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="8" t="n">
         <f aca="false">E5+E12+E19</f>
         <v>436735</v>
       </c>
@@ -3732,19 +3821,19 @@
       <c r="A28" s="5" t="n">
         <v>29733</v>
       </c>
-      <c r="B28" s="7" t="n">
+      <c r="B28" s="8" t="n">
         <f aca="false">B6+B13+B20</f>
         <v>238063</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="8" t="n">
         <f aca="false">C6+C13+C20</f>
         <v>238135</v>
       </c>
-      <c r="D28" s="7" t="n">
+      <c r="D28" s="8" t="n">
         <f aca="false">D6+D13+D20</f>
         <v>238207</v>
       </c>
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="8" t="n">
         <f aca="false">E6+E13+E20</f>
         <v>238279</v>
       </c>
@@ -3753,31 +3842,31 @@
       <c r="A29" s="5" t="n">
         <v>26235</v>
       </c>
-      <c r="B29" s="7" t="n">
+      <c r="B29" s="8" t="n">
         <f aca="false">B7+B14+B21</f>
         <v>210079</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="8" t="n">
         <f aca="false">C7+C14+C21</f>
         <v>210151</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="8" t="n">
         <f aca="false">D7+D14+D21</f>
         <v>210223</v>
       </c>
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="8" t="n">
         <f aca="false">E7+E14+E21</f>
         <v>210295</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
-        <v>9</v>
+      <c r="A38" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
@@ -3788,43 +3877,43 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>3</v>
@@ -3832,51 +3921,51 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>3</v>
@@ -3885,12 +3974,12 @@
         <v>1</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>14</v>
@@ -3899,12 +3988,12 @@
         <v>1</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
-        <v>22</v>
+      <c r="A52" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3912,10 +4001,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,10 +4012,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3937,10 +4026,10 @@
         <v>1</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,12 +4040,12 @@
         <v>1</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
-        <v>26</v>
+      <c r="A59" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,10 +4053,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3975,7 +4064,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,10 +4072,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4013,11 +4102,11 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R31" activeCellId="0" sqref="R31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.38"/>
@@ -4065,64 +4154,67 @@
       <c r="A4" s="5" t="n">
         <v>38160</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="10" t="n">
         <f aca="false">H28*(3*(10*$A4+11*B$3*$A4+12*B$3)+15*B$3+14*B$3*$A4+13*$A4+15)</f>
         <v>52280370</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <f aca="false">I28*(3*(10*$A4+11*C$3*$A4+12*C$3)+15*C$3+14*C$3*$A4+13*$A4+15)</f>
         <v>70216080</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <f aca="false">J28*(3*(10*$A4+11*D$3*$A4+12*D$3)+15*D$3+14*D$3*$A4+13*$A4+15)</f>
         <v>132227685</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="10" t="n">
         <f aca="false">K28*(3*(10*$A4+11*E$3*$A4+12*E$3)+15*E$3+14*E$3*$A4+13*$A4+15)</f>
         <v>201566250</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>54540</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <f aca="false">H29*(3*(10*$A5+11*B$3*$A5+12*B$3)+15*B$3+14*B$3*$A5+13*$A5+15)</f>
         <v>44832582</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <f aca="false">I29*(3*(10*$A5+11*C$3*$A5+12*C$3)+15*C$3+14*C$3*$A5+13*$A5+15)</f>
         <v>110390808</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <f aca="false">J29*(3*(10*$A5+11*D$3*$A5+12*D$3)+15*D$3+14*D$3*$A5+13*$A5+15)</f>
         <v>277177098</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="10" t="n">
         <f aca="false">K29*(3*(10*$A5+11*E$3*$A5+12*E$3)+15*E$3+14*E$3*$A5+13*$A5+15)</f>
         <v>181948680</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>29733</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <f aca="false">H30*(3*(10*$A6+11*B$3*$A6+12*B$3)+15*B$3+14*B$3*$A6+13*$A6+15)</f>
         <v>44808918</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <f aca="false">I30*(3*(10*$A6+11*C$3*$A6+12*C$3)+15*C$3+14*C$3*$A6+13*$A6+15)</f>
         <v>49239360</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <f aca="false">J30*(3*(10*$A6+11*D$3*$A6+12*D$3)+15*D$3+14*D$3*$A6+13*$A6+15)</f>
         <v>89291046</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <f aca="false">K30*(3*(10*$A6+11*E$3*$A6+12*E$3)+15*E$3+14*E$3*$A6+13*$A6+15)</f>
         <v>115724616</v>
       </c>
@@ -4131,26 +4223,26 @@
       <c r="A7" s="5" t="n">
         <v>26235</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <f aca="false">H31*(3*(10*$A7+11*B$3*$A7+12*B$3)+15*B$3+14*B$3*$A7+13*$A7+15)</f>
         <v>17971560</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <f aca="false">I31*(3*(10*$A7+11*C$3*$A7+12*C$3)+15*C$3+14*C$3*$A7+13*$A7+15)</f>
         <v>48274080</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <f aca="false">J31*(3*(10*$A7+11*D$3*$A7+12*D$3)+15*D$3+14*D$3*$A7+13*$A7+15)</f>
         <v>78786552</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="10" t="n">
         <f aca="false">K31*(3*(10*$A7+11*E$3*$A7+12*E$3)+15*E$3+14*E$3*$A7+13*$A7+15)</f>
         <v>65642400</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4187,64 +4279,67 @@
       <c r="A11" s="5" t="n">
         <v>38160</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="10" t="n">
         <f aca="false">H28*(3*(3*B$10*$A11+2*$A11+2*B$10)+B$10*$A11+4*B$10+7*$A11+1)</f>
         <v>12593010</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="10" t="n">
         <f aca="false">I28*(3*(3*C$10*$A11+2*$A11+2*C$10)+C$10*$A11+4*C$10+7*$A11+1)</f>
         <v>16409110</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="10" t="n">
         <f aca="false">J28*(3*(3*D$10*$A11+2*$A11+2*D$10)+D$10*$A11+4*D$10+7*$A11+1)</f>
         <v>30337815</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="10" t="n">
         <f aca="false">K28*(3*(3*E$10*$A11+2*$A11+2*E$10)+E$10*$A11+4*E$10+7*$A11+1)</f>
         <v>45678489</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>54540</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <f aca="false">H29*(3*(3*B$10*$A12+2*$A12+2*B$10)+B$10*$A12+4*B$10+7*$A12+1)</f>
         <v>10799046</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="10" t="n">
         <f aca="false">I29*(3*(3*C$10*$A12+2*$A12+2*C$10)+C$10*$A12+4*C$10+7*$A12+1)</f>
         <v>25797761</v>
       </c>
-      <c r="D12" s="9" t="n">
+      <c r="D12" s="10" t="n">
         <f aca="false">J29*(3*(3*D$10*$A12+2*$A12+2*D$10)+D$10*$A12+4*D$10+7*$A12+1)</f>
         <v>63594542</v>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="E12" s="10" t="n">
         <f aca="false">K29*(3*(3*E$10*$A12+2*$A12+2*E$10)+E$10*$A12+4*E$10+7*$A12+1)</f>
         <v>41232852</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>29733</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="10" t="n">
         <f aca="false">H30*(3*(3*B$10*$A13+2*$A13+2*B$10)+B$10*$A13+4*B$10+7*$A13+1)</f>
         <v>10793310</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="10" t="n">
         <f aca="false">I30*(3*(3*C$10*$A13+2*$A13+2*C$10)+C$10*$A13+4*C$10+7*$A13+1)</f>
         <v>11506950</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="10" t="n">
         <f aca="false">J30*(3*(3*D$10*$A13+2*$A13+2*D$10)+D$10*$A13+4*D$10+7*$A13+1)</f>
         <v>20486570</v>
       </c>
-      <c r="E13" s="9" t="n">
+      <c r="E13" s="10" t="n">
         <f aca="false">K30*(3*(3*E$10*$A13+2*$A13+2*E$10)+E$10*$A13+4*E$10+7*$A13+1)</f>
         <v>26225220</v>
       </c>
@@ -4253,26 +4348,26 @@
       <c r="A14" s="5" t="n">
         <v>26235</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="10" t="n">
         <f aca="false">H31*(3*(3*B$10*$A14+2*$A14+2*B$10)+B$10*$A14+4*B$10+7*$A14+1)</f>
         <v>4328880</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <f aca="false">I31*(3*(3*C$10*$A14+2*$A14+2*C$10)+C$10*$A14+4*C$10+7*$A14+1)</f>
         <v>11281360</v>
       </c>
-      <c r="D14" s="9" t="n">
+      <c r="D14" s="10" t="n">
         <f aca="false">J31*(3*(3*D$10*$A14+2*$A14+2*D$10)+D$10*$A14+4*D$10+7*$A14+1)</f>
         <v>18076448</v>
       </c>
-      <c r="E14" s="9" t="n">
+      <c r="E14" s="10" t="n">
         <f aca="false">K31*(3*(3*E$10*$A14+2*$A14+2*E$10)+E$10*$A14+4*E$10+7*$A14+1)</f>
         <v>14875704</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4289,7 +4384,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="n">
@@ -4309,92 +4404,95 @@
       <c r="A18" s="5" t="n">
         <v>38160</v>
       </c>
-      <c r="B18" s="9" t="n">
-        <f aca="false">H28*(3*(B$17+B$17+$A18)+2*(B$17+$A18)+3*(B$17+$A18)+1)</f>
-        <v>3053030</v>
-      </c>
-      <c r="C18" s="9" t="n">
-        <f aca="false">I28*(3*(C$17+C$17+$A18)+2*(C$17+$A18)+3*(C$17+$A18)+1)</f>
-        <v>3053140</v>
-      </c>
-      <c r="D18" s="9" t="n">
-        <f aca="false">J28*(3*(D$17+D$17+$A18)+2*(D$17+$A18)+3*(D$17+$A18)+1)</f>
-        <v>4579875</v>
-      </c>
-      <c r="E18" s="9" t="n">
-        <f aca="false">K28*(3*(E$17+E$17+$A18)+2*(E$17+$A18)+3*(E$17+$A18)+1)</f>
-        <v>5801384</v>
+      <c r="B18" s="10" t="n">
+        <f aca="false">H28*(3*(B$17*$A18+B$17+$A18)+2*(B$17+$A18)+3*(B$17+$A18)+1)</f>
+        <v>5342570</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <f aca="false">I28*(3*(C$17*$A18+C$17+$A18)+2*(C$17+$A18)+3*(C$17+$A18)+1)</f>
+        <v>6487450</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <f aca="false">J28*(3*(D$17*$A18+D$17+$A18)+2*(D$17+$A18)+3*(D$17+$A18)+1)</f>
+        <v>11448495</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <f aca="false">K28*(3*(E$17*$A18+E$17+$A18)+2*(E$17+$A18)+3*(E$17+$A18)+1)</f>
+        <v>16676699</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>54540</v>
       </c>
-      <c r="B19" s="9" t="n">
-        <f aca="false">H29*(3*(B$17+B$17+$A19)+2*(B$17+$A19)+3*(B$17+$A19)+1)</f>
-        <v>2618058</v>
-      </c>
-      <c r="C19" s="9" t="n">
-        <f aca="false">I29*(3*(C$17+C$17+$A19)+2*(C$17+$A19)+3*(C$17+$A19)+1)</f>
-        <v>4799894</v>
-      </c>
-      <c r="D19" s="9" t="n">
-        <f aca="false">J29*(3*(D$17+D$17+$A19)+2*(D$17+$A19)+3*(D$17+$A19)+1)</f>
-        <v>9600030</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <f aca="false">K29*(3*(E$17+E$17+$A19)+2*(E$17+$A19)+3*(E$17+$A19)+1)</f>
-        <v>5236512</v>
+      <c r="B19" s="10" t="n">
+        <f aca="false">H29*(3*(B$17*$A19+B$17+$A19)+2*(B$17+$A19)+3*(B$17+$A19)+1)</f>
+        <v>4581462</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <f aca="false">I29*(3*(C$17*$A19+C$17+$A19)+2*(C$17+$A19)+3*(C$17+$A19)+1)</f>
+        <v>10199255</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <f aca="false">J29*(3*(D$17*$A19+D$17+$A19)+2*(D$17+$A19)+3*(D$17+$A19)+1)</f>
+        <v>23998326</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <f aca="false">K29*(3*(E$17*$A19+E$17+$A19)+2*(E$17+$A19)+3*(E$17+$A19)+1)</f>
+        <v>15053532</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>29733</v>
       </c>
-      <c r="B20" s="9" t="n">
-        <f aca="false">H30*(3*(B$17+B$17+$A20)+2*(B$17+$A20)+3*(B$17+$A20)+1)</f>
-        <v>2616757</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <f aca="false">I30*(3*(C$17+C$17+$A20)+2*(C$17+$A20)+3*(C$17+$A20)+1)</f>
-        <v>2141082</v>
-      </c>
-      <c r="D20" s="9" t="n">
-        <f aca="false">J30*(3*(D$17+D$17+$A20)+2*(D$17+$A20)+3*(D$17+$A20)+1)</f>
-        <v>3092817</v>
-      </c>
-      <c r="E20" s="9" t="n">
-        <f aca="false">K30*(3*(E$17+E$17+$A20)+2*(E$17+$A20)+3*(E$17+$A20)+1)</f>
-        <v>3330880</v>
+      <c r="B20" s="10" t="n">
+        <f aca="false">H30*(3*(B$17*$A20+B$17+$A20)+2*(B$17+$A20)+3*(B$17+$A20)+1)</f>
+        <v>4579069</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <f aca="false">I30*(3*(C$17*$A20+C$17+$A20)+2*(C$17+$A20)+3*(C$17+$A20)+1)</f>
+        <v>4549374</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <f aca="false">J30*(3*(D$17*$A20+D$17+$A20)+2*(D$17+$A20)+3*(D$17+$A20)+1)</f>
+        <v>7731009</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <f aca="false">K30*(3*(E$17*$A20+E$17+$A20)+2*(E$17+$A20)+3*(E$17+$A20)+1)</f>
+        <v>9574600</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>26235</v>
       </c>
-      <c r="B21" s="9" t="n">
-        <f aca="false">H31*(3*(B$17+B$17+$A21)+2*(B$17+$A21)+3*(B$17+$A21)+1)</f>
-        <v>1049515</v>
-      </c>
-      <c r="C21" s="9" t="n">
-        <f aca="false">I31*(3*(C$17+C$17+$A21)+2*(C$17+$A21)+3*(C$17+$A21)+1)</f>
-        <v>2099140</v>
-      </c>
-      <c r="D21" s="9" t="n">
-        <f aca="false">J31*(3*(D$17+D$17+$A21)+2*(D$17+$A21)+3*(D$17+$A21)+1)</f>
-        <v>2729025</v>
-      </c>
-      <c r="E21" s="9" t="n">
-        <f aca="false">K31*(3*(E$17+E$17+$A21)+2*(E$17+$A21)+3*(E$17+$A21)+1)</f>
-        <v>1889424</v>
+      <c r="B21" s="10" t="n">
+        <f aca="false">H31*(3*(B$17*$A21+B$17+$A21)+2*(B$17+$A21)+3*(B$17+$A21)+1)</f>
+        <v>1836535</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <f aca="false">I31*(3*(C$17*$A21+C$17+$A21)+2*(C$17+$A21)+3*(C$17+$A21)+1)</f>
+        <v>4460200</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <f aca="false">J31*(3*(D$17*$A21+D$17+$A21)+2*(D$17+$A21)+3*(D$17+$A21)+1)</f>
+        <v>6821529</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <f aca="false">K31*(3*(E$17*$A21+E$17+$A21)+2*(E$17+$A21)+3*(E$17+$A21)+1)</f>
+        <v>5431014</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4403,15 +4501,15 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="5" t="n">
@@ -4431,62 +4529,62 @@
       <c r="A26" s="5" t="n">
         <v>38160</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="12" t="n">
         <f aca="false">B4+B11+B18</f>
-        <v>67926410</v>
-      </c>
-      <c r="C26" s="11" t="n">
+        <v>70215950</v>
+      </c>
+      <c r="C26" s="12" t="n">
         <f aca="false">C4+C11+C18</f>
-        <v>89678330</v>
-      </c>
-      <c r="D26" s="11" t="n">
+        <v>93112640</v>
+      </c>
+      <c r="D26" s="12" t="n">
         <f aca="false">D4+D11+D18</f>
-        <v>167145375</v>
-      </c>
-      <c r="E26" s="11" t="n">
+        <v>174013995</v>
+      </c>
+      <c r="E26" s="12" t="n">
         <f aca="false">E4+E11+E18</f>
-        <v>253046123</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+        <v>263921438</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
         <v>54540</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="12" t="n">
         <f aca="false">B5+B12+B19</f>
-        <v>58249686</v>
-      </c>
-      <c r="C27" s="11" t="n">
+        <v>60213090</v>
+      </c>
+      <c r="C27" s="12" t="n">
         <f aca="false">C5+C12+C19</f>
-        <v>140988463</v>
-      </c>
-      <c r="D27" s="11" t="n">
+        <v>146387824</v>
+      </c>
+      <c r="D27" s="12" t="n">
         <f aca="false">D5+D12+D19</f>
-        <v>350371670</v>
-      </c>
-      <c r="E27" s="11" t="n">
+        <v>364769966</v>
+      </c>
+      <c r="E27" s="12" t="n">
         <f aca="false">E5+E12+E19</f>
-        <v>228418044</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I27" s="13" t="n">
+        <v>238235064</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="J27" s="13" t="n">
+      <c r="J27" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K27" s="14" t="n">
+      <c r="K27" s="15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4494,35 +4592,35 @@
       <c r="A28" s="5" t="n">
         <v>29733</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="12" t="n">
         <f aca="false">B6+B13+B20</f>
-        <v>58218985</v>
-      </c>
-      <c r="C28" s="11" t="n">
+        <v>60181297</v>
+      </c>
+      <c r="C28" s="12" t="n">
         <f aca="false">C6+C13+C20</f>
-        <v>62887392</v>
-      </c>
-      <c r="D28" s="11" t="n">
+        <v>65295684</v>
+      </c>
+      <c r="D28" s="12" t="n">
         <f aca="false">D6+D13+D20</f>
-        <v>112870433</v>
-      </c>
-      <c r="E28" s="11" t="n">
+        <v>117508625</v>
+      </c>
+      <c r="E28" s="12" t="n">
         <f aca="false">E6+E13+E20</f>
-        <v>145280716</v>
-      </c>
-      <c r="G28" s="12" t="n">
+        <v>151524436</v>
+      </c>
+      <c r="G28" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="H28" s="15" t="n">
+      <c r="H28" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="I28" s="16" t="n">
+      <c r="I28" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="J28" s="16" t="n">
+      <c r="J28" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="K28" s="17" t="n">
+      <c r="K28" s="18" t="n">
         <v>19</v>
       </c>
     </row>
@@ -4530,83 +4628,83 @@
       <c r="A29" s="5" t="n">
         <v>26235</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="12" t="n">
         <f aca="false">B7+B14+B21</f>
-        <v>23349955</v>
-      </c>
-      <c r="C29" s="11" t="n">
+        <v>24136975</v>
+      </c>
+      <c r="C29" s="12" t="n">
         <f aca="false">C7+C14+C21</f>
-        <v>61654580</v>
-      </c>
-      <c r="D29" s="11" t="n">
+        <v>64015640</v>
+      </c>
+      <c r="D29" s="12" t="n">
         <f aca="false">D7+D14+D21</f>
-        <v>99592025</v>
-      </c>
-      <c r="E29" s="11" t="n">
+        <v>103684529</v>
+      </c>
+      <c r="E29" s="12" t="n">
         <f aca="false">E7+E14+E21</f>
-        <v>82407528</v>
-      </c>
-      <c r="G29" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="H29" s="15" t="n">
+        <v>85949118</v>
+      </c>
+      <c r="G29" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H29" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="I29" s="16" t="n">
+      <c r="I29" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="J29" s="16" t="n">
+      <c r="J29" s="17" t="n">
         <v>22</v>
       </c>
-      <c r="K29" s="17" t="n">
+      <c r="K29" s="18" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G30" s="12" t="n">
+      <c r="G30" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="H30" s="15" t="n">
+      <c r="H30" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="I30" s="16" t="n">
+      <c r="I30" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="J30" s="16" t="n">
+      <c r="J30" s="17" t="n">
         <v>13</v>
       </c>
-      <c r="K30" s="17" t="n">
+      <c r="K30" s="18" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="12" t="n">
+      <c r="G31" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H31" s="15" t="n">
+      <c r="H31" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="I31" s="16" t="n">
+      <c r="I31" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="J31" s="16" t="n">
+      <c r="J31" s="17" t="n">
         <v>13</v>
       </c>
-      <c r="K31" s="17" t="n">
+      <c r="K31" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
-        <v>9</v>
+      <c r="A37" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4717,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4627,10 +4725,10 @@
         <v>6</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4638,7 +4736,7 @@
         <v>3</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4744,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,7 +4752,7 @@
         <v>3</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,12 +4763,12 @@
         <v>2</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
@@ -4684,7 +4782,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>3</v>
@@ -4706,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>2</v>
@@ -4717,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>2</v>
@@ -4728,7 +4826,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>2</v>
@@ -4739,10 +4837,10 @@
         <v>3</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>2</v>
@@ -4753,10 +4851,10 @@
         <v>8</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>2</v>
@@ -4767,7 +4865,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>2</v>
@@ -4778,7 +4876,7 @@
         <v>4</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>2</v>
@@ -4802,7 +4900,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>3</v>
@@ -4829,7 +4927,7 @@
         <v>3</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>2</v>
@@ -4840,7 +4938,7 @@
         <v>7</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>2</v>
@@ -4856,7 +4954,7 @@
         <v>3</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4864,7 +4962,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4872,7 +4970,7 @@
         <v>3</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4880,10 +4978,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4891,32 +4989,32 @@
         <v>9</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
-        <v>22</v>
+      <c r="A70" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +5043,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>2</v>
@@ -4956,10 +5054,10 @@
         <v>1</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>2</v>
@@ -4970,10 +5068,10 @@
         <v>2</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>2</v>
@@ -5008,7 +5106,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>2</v>
@@ -5019,7 +5117,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>2</v>
@@ -5030,7 +5128,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5038,10 +5136,10 @@
         <v>1</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,18 +5147,18 @@
         <v>1</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8" t="s">
-        <v>26</v>
+      <c r="A88" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5068,10 +5166,10 @@
         <v>1</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,7 +5180,7 @@
         <v>2</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5090,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>2</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5104,16 +5202,16 @@
         <v>1</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E92" s="0" t="s">
         <v>2</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5121,13 +5219,13 @@
         <v>1</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>2</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5138,7 +5236,7 @@
         <v>2</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5162,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>2</v>
@@ -5173,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5181,7 +5279,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5189,10 +5287,10 @@
         <v>1</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>